<commit_message>
Update result.xlsx by Ruofan
</commit_message>
<xml_diff>
--- a/lstm_test/result.xlsx
+++ b/lstm_test/result.xlsx
@@ -249,7 +249,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -300,13 +300,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.00114351057747</v>
+        <f aca="false">1-0.00114351057747</f>
+        <v>0.99885648942253</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.0108695652174</v>
+        <f aca="false">1-0.0108695652174</f>
+        <v>0.9891304347826</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.0502702702703</v>
+        <f aca="false">1-0.0502702702703</f>
+        <v>0.9497297297297</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>10</v>
@@ -329,13 +332,16 @@
         <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.00664451827243</v>
+        <f aca="false">1-0.00664451827243</f>
+        <v>0.99335548172757</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.027027027027</v>
+        <f aca="false">1-0.027027027027</f>
+        <v>0.972972972973</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.0489887640449</v>
+        <f aca="false">1-0.0489887640449</f>
+        <v>0.9510112359551</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
@@ -358,13 +364,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.00069060773480667</v>
+        <f aca="false">1-0.00069060773480667</f>
+        <v>0.999309392265193</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.0526315789473685</v>
+        <f aca="false">1-0.0526315789473685</f>
+        <v>0.947368421052632</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.0606653620352251</v>
+        <f aca="false">1-0.0606653620352251</f>
+        <v>0.939334637964775</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>14</v>
@@ -387,13 +396,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.00190566936636</v>
+        <f aca="false">1-0.00190566936636</f>
+        <v>0.99809433063364</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.0272727272727</v>
+        <f aca="false">1-0.0272727272727</f>
+        <v>0.9727272727273</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.0691056910569</v>
+        <f aca="false">1-0.0691056910569</f>
+        <v>0.9308943089431</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>16</v>
@@ -416,13 +428,16 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.0460829493088</v>
+        <f aca="false">1-0.0460829493088</f>
+        <v>0.9539170506912</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>18</v>
@@ -445,13 +460,16 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.000473709142586487</v>
+        <f aca="false">1-0.000473709142586487</f>
+        <v>0.999526290857414</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.036036036036036</v>
+        <f aca="false">1-0.036036036036036</f>
+        <v>0.963963963963964</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.0613718411552346</v>
+        <f aca="false">1-0.0613718411552346</f>
+        <v>0.938628158844765</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>20</v>
@@ -474,13 +492,16 @@
         <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.0833333333333</v>
+        <f aca="false">1-0.0833333333333</f>
+        <v>0.9166666666667</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.0857142857143</v>
+        <f aca="false">1-0.0857142857143</f>
+        <v>0.9142857142857</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>22</v>
@@ -503,13 +524,16 @@
         <v>23</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.0180180180180181</v>
+        <f aca="false">1-0.0180180180180181</f>
+        <v>0.981981981981982</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.0470588235294118</v>
+        <f aca="false">1-0.0470588235294118</f>
+        <v>0.952941176470588</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>24</v>
@@ -532,13 +556,16 @@
         <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.0159726183685</v>
+        <f aca="false">1-0.0159726183685</f>
+        <v>0.9840273816315</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.0108695652174</v>
+        <f aca="false">1-0.0108695652174</f>
+        <v>0.9891304347826</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.0573903627504</v>
+        <f aca="false">1-0.0573903627504</f>
+        <v>0.9426096372496</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>26</v>
@@ -561,13 +588,16 @@
         <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.00996677740864</v>
+        <f aca="false">1-0.00996677740864</f>
+        <v>0.99003322259136</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.0540540540541</v>
+        <f aca="false">1-0.0540540540541</f>
+        <v>0.9459459459459</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.0572587917042</v>
+        <f aca="false">1-0.0572587917042</f>
+        <v>0.9427412082958</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>28</v>
@@ -590,13 +620,16 @@
         <v>29</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.0833333333333</v>
+        <f aca="false">1-0.0833333333333</f>
+        <v>0.9166666666667</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.065306122449</v>
+        <f aca="false">1-0.065306122449</f>
+        <v>0.934693877551</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>30</v>
@@ -619,13 +652,16 @@
         <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.00709219858156</v>
+        <f aca="false">1-0.00709219858156</f>
+        <v>0.99290780141844</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.0753424657534</v>
+        <f aca="false">1-0.0753424657534</f>
+        <v>0.9246575342466</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>32</v>
@@ -648,13 +684,16 @@
         <v>33</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.00429184549356</v>
+        <f aca="false">1-0.00429184549356</f>
+        <v>0.99570815450644</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.0491803278689</v>
+        <f aca="false">1-0.0491803278689</f>
+        <v>0.9508196721311</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>34</v>
@@ -677,13 +716,16 @@
         <v>35</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.0456621004566</v>
+        <f aca="false">1-0.0456621004566</f>
+        <v>0.9543378995434</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>36</v>
@@ -706,13 +748,16 @@
         <v>37</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.093131548312</v>
+        <f aca="false">1-0.093131548312</f>
+        <v>0.906868451688</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.121546961326</v>
+        <f aca="false">1-0.121546961326</f>
+        <v>0.878453038674</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.105918141593</v>
+        <f aca="false">1-0.105918141593</f>
+        <v>0.894081858407</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>38</v>
@@ -735,13 +780,16 @@
         <v>39</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.00189753320683</v>
+        <f aca="false">1-0.00189753320683</f>
+        <v>0.99810246679317</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.0630630630631</v>
+        <f aca="false">1-0.0630630630631</f>
+        <v>0.9369369369369</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.0803974706414</v>
+        <f aca="false">1-0.0803974706414</f>
+        <v>0.9196025293586</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>40</v>
@@ -764,13 +812,16 @@
         <v>41</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.0462962962963</v>
+        <f aca="false">1-0.0462962962963</f>
+        <v>0.9537037037037</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>42</v>
@@ -793,13 +844,16 @@
         <v>43</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1-0</f>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.181818181818</v>
+        <f aca="false">1-0.181818181818</f>
+        <v>0.818181818182</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.0601851851852</v>
+        <f aca="false">1-0.0601851851852</f>
+        <v>0.9398148148148</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>44</v>

</xml_diff>